<commit_message>
Changed output name in XLSX files for HaunStage
</commit_message>
<xml_diff>
--- a/Tests/Validation/Barley/Observations/CPT.xlsx
+++ b/Tests/Validation/Barley/Observations/CPT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHubRepos\ApsimX\Prototypes\Barley\Observations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ApsimX\Tests\Validation\Barley\Observations\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAAD84F-7602-45C9-81A5-D42DE0BF88FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -272,13 +273,13 @@
     <t>CPTCultVORTEXSD2005-12-05</t>
   </si>
   <si>
-    <t>Barley.Structure.HaunStage.Value()</t>
+    <t>Barley.Phenology.HaunStage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -601,11 +602,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>